<commit_message>
update food secure fraction
</commit_message>
<xml_diff>
--- a/Input_LiST_Bangladesh_2016.xlsx
+++ b/Input_LiST_Bangladesh_2016.xlsx
@@ -563,7 +563,7 @@
         <v>5</v>
       </c>
       <c r="B5" s="2">
-        <v>0.44</v>
+        <v>0.4</v>
       </c>
     </row>
     <row r="6">
@@ -2007,7 +2007,7 @@
         <v>1.0</v>
       </c>
       <c r="F4" s="5">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="G4" s="5">
         <v>0.0</v>
@@ -2025,15 +2025,14 @@
       </c>
       <c r="D5" s="5" t="str">
         <f>demographics!$B$5</f>
-        <v>0.44</v>
+        <v>0.4</v>
       </c>
       <c r="E5" s="5" t="str">
         <f>demographics!$B$5</f>
-        <v>0.44</v>
-      </c>
-      <c r="F5" s="5" t="str">
-        <f>demographics!$B$5</f>
-        <v>0.44</v>
+        <v>0.4</v>
+      </c>
+      <c r="F5" s="5">
+        <v>0.0</v>
       </c>
       <c r="G5" s="5">
         <v>0.0</v>
@@ -2266,15 +2265,15 @@
       </c>
       <c r="C3" s="18" t="str">
         <f>demographics!$B$5</f>
-        <v>0.44</v>
+        <v>0.40</v>
       </c>
       <c r="D3" s="18" t="str">
         <f>demographics!$B$5</f>
-        <v>0.44</v>
+        <v>0.40</v>
       </c>
       <c r="E3" s="18" t="str">
         <f>demographics!$B$5</f>
-        <v>0.44</v>
+        <v>0.40</v>
       </c>
       <c r="F3" s="18">
         <v>0.0</v>

</xml_diff>

<commit_message>
update food insecure fraction
</commit_message>
<xml_diff>
--- a/Input_LiST_Bangladesh_2016.xlsx
+++ b/Input_LiST_Bangladesh_2016.xlsx
@@ -563,7 +563,7 @@
         <v>5</v>
       </c>
       <c r="B5" s="2">
-        <v>0.4</v>
+        <v>0.44</v>
       </c>
     </row>
     <row r="6">
@@ -2025,11 +2025,11 @@
       </c>
       <c r="D5" s="5" t="str">
         <f>demographics!$B$5</f>
-        <v>0.4</v>
+        <v>0.44</v>
       </c>
       <c r="E5" s="5" t="str">
         <f>demographics!$B$5</f>
-        <v>0.4</v>
+        <v>0.44</v>
       </c>
       <c r="F5" s="5">
         <v>0.0</v>
@@ -2265,15 +2265,15 @@
       </c>
       <c r="C3" s="18" t="str">
         <f>demographics!$B$5</f>
-        <v>0.40</v>
+        <v>0.44</v>
       </c>
       <c r="D3" s="18" t="str">
         <f>demographics!$B$5</f>
-        <v>0.40</v>
+        <v>0.44</v>
       </c>
       <c r="E3" s="18" t="str">
         <f>demographics!$B$5</f>
-        <v>0.40</v>
+        <v>0.44</v>
       </c>
       <c r="F3" s="18">
         <v>0.0</v>

</xml_diff>

<commit_message>
remove bad reference to current year births
</commit_message>
<xml_diff>
--- a/Input_LiST_Bangladesh_2016.xlsx
+++ b/Input_LiST_Bangladesh_2016.xlsx
@@ -2083,122 +2083,113 @@
     </row>
     <row r="2">
       <c r="A2" s="5">
-        <v>2016.0</v>
-      </c>
-      <c r="B2" s="6" t="str">
-        <f>demographics!$B$3</f>
-        <v>3,030,000</v>
+        <v>2017.0</v>
+      </c>
+      <c r="B2" s="6">
+        <v>3010000.0</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="5">
-        <v>2017.0</v>
+        <v>2018.0</v>
       </c>
       <c r="B3" s="6">
-        <v>3010000.0</v>
+        <v>2980000.0</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="5">
-        <v>2018.0</v>
+        <v>2019.0</v>
       </c>
       <c r="B4" s="6">
-        <v>2980000.0</v>
+        <v>2960000.0</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="5">
-        <v>2019.0</v>
+        <v>2020.0</v>
       </c>
       <c r="B5" s="6">
-        <v>2960000.0</v>
+        <v>2930000.0</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="5">
-        <v>2020.0</v>
+        <v>2021.0</v>
       </c>
       <c r="B6" s="6">
-        <v>2930000.0</v>
+        <v>2900000.0</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="5">
-        <v>2021.0</v>
+        <v>2022.0</v>
       </c>
       <c r="B7" s="6">
-        <v>2900000.0</v>
+        <v>2870000.0</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="5">
-        <v>2022.0</v>
+        <v>2023.0</v>
       </c>
       <c r="B8" s="6">
-        <v>2870000.0</v>
+        <v>2840000.0</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="5">
-        <v>2023.0</v>
+        <v>2024.0</v>
       </c>
       <c r="B9" s="6">
-        <v>2840000.0</v>
+        <v>2810000.0</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="5">
-        <v>2024.0</v>
+        <v>2025.0</v>
       </c>
       <c r="B10" s="6">
-        <v>2810000.0</v>
+        <v>2780000.0</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="5">
-        <v>2025.0</v>
+        <v>2026.0</v>
       </c>
       <c r="B11" s="6">
-        <v>2780000.0</v>
+        <v>2740000.0</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="5">
-        <v>2026.0</v>
+        <v>2027.0</v>
       </c>
       <c r="B12" s="6">
-        <v>2740000.0</v>
+        <v>2710000.0</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="5">
-        <v>2027.0</v>
+        <v>2028.0</v>
       </c>
       <c r="B13" s="6">
-        <v>2710000.0</v>
+        <v>2670000.0</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="5">
-        <v>2028.0</v>
+        <v>2029.0</v>
       </c>
       <c r="B14" s="6">
-        <v>2670000.0</v>
+        <v>2640000.0</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="5">
-        <v>2029.0</v>
+        <v>2030.0</v>
       </c>
       <c r="B15" s="6">
-        <v>2640000.0</v>
-      </c>
-    </row>
-    <row r="16">
-      <c r="A16" s="5">
-        <v>2030.0</v>
-      </c>
-      <c r="B16" s="6">
         <v>2600000.0</v>
       </c>
     </row>

</xml_diff>